<commit_message>
Update excel stats files
</commit_message>
<xml_diff>
--- a/Analysis/BGLStats.xlsx
+++ b/Analysis/BGLStats.xlsx
@@ -8,24 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\MGL870-TP2-Remise\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1682B972-AF9B-4165-A523-C7B440150982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC447E2E-E33A-4E53-927D-B3E625E934DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13176" yWindow="1080" windowWidth="27624" windowHeight="20940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Stats" sheetId="1" r:id="rId1"/>
+    <sheet name="Stats 2" sheetId="2" r:id="rId2"/>
     <sheet name="AUC" sheetId="3" r:id="rId3"/>
+    <sheet name="RF+RL Traning" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$6:$B$46</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$6:$C$46</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$6:$B$46</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$6:$C$46</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet2!$B$6:$B$46</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet2!$D$6:$D$46</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet2!$B$6:$B$46</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet2!$D$6:$D$46</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Stats!$B$6:$B$46</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Stats!$C$6:$C$46</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Stats!$B$6:$B$46</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Stats!$C$6:$C$46</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Stats 2'!$B$6:$B$46</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Stats 2'!$D$6:$D$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="60">
   <si>
     <t>APPALLOC</t>
   </si>
@@ -216,6 +215,18 @@
   </si>
   <si>
     <t>Confiance</t>
+  </si>
+  <si>
+    <t>Metric Query</t>
+  </si>
+  <si>
+    <t>RF Score</t>
+  </si>
+  <si>
+    <t>RL Score</t>
+  </si>
+  <si>
+    <t>F1-Score</t>
   </si>
 </sst>
 </file>
@@ -253,7 +264,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,6 +319,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -321,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -366,6 +395,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -542,7 +580,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$6:$B$46</c:f>
+              <c:f>Stats!$B$6:$B$46</c:f>
               <c:strCache>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
@@ -673,7 +711,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$C$46</c:f>
+              <c:f>Stats!$C$6:$C$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -1103,10 +1141,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.4</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4834,8 +4872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB05F75-7C24-44B7-9C4B-11B76B25B82F}">
   <dimension ref="B4:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5357,4 +5395,250 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{925387E9-A761-43C7-A3F6-A7F0D6717FC1}">
+  <dimension ref="B5:E26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B5" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B5:E5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update analysis excel files
</commit_message>
<xml_diff>
--- a/Analysis/BGLStats.xlsx
+++ b/Analysis/BGLStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\MGL870-TP2-Remise\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC447E2E-E33A-4E53-927D-B3E625E934DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D04511-2ABC-4B51-A298-CEED162758DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,10 +21,19 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Stats!$B$6:$B$46</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Stats!$C$6:$C$46</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'RF+RL Traning'!$E$6</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'RF+RL Traning'!$E$7:$E$36</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'RF+RL Traning'!$B$7:$B$36</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'RF+RL Traning'!$C$6</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'RF+RL Traning'!$C$7:$C$36</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Stats!$B$6:$B$46</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Stats!$C$6:$C$46</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">'Stats 2'!$B$6:$B$46</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">'Stats 2'!$D$6:$D$46</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'RF+RL Traning'!$B$7:$B$36</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'RF+RL Traning'!$C$6</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'RF+RL Traning'!$C$7:$C$36</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'RF+RL Traning'!$D$7:$D$36</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="67">
   <si>
     <t>APPALLOC</t>
   </si>
@@ -228,6 +237,27 @@
   <si>
     <t>F1-Score</t>
   </si>
+  <si>
+    <t>R-Square</t>
+  </si>
+  <si>
+    <t>5000 th 50</t>
+  </si>
+  <si>
+    <t>5000 th 15</t>
+  </si>
+  <si>
+    <t>4500 th 15</t>
+  </si>
+  <si>
+    <t>3000 th 45</t>
+  </si>
+  <si>
+    <t>2000 th 50</t>
+  </si>
+  <si>
+    <t>1000 th 50</t>
+  </si>
 </sst>
 </file>
 
@@ -391,19 +421,19 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1027,10 +1057,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1109,10 +1139,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1214,6 +1244,124 @@
         <cx:tickLabels/>
       </cx:axis>
     </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx4.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.9</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.8</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.9</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.11</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Performances de RF et RL - BGL 5M - 80%-20% - Alarme </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>KERNDTLB</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{081407F1-00F4-4940-A706-C1CA52CC8A8E}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.7</cx:f>
+              <cx:v>RF Score</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataLabels>
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000001-DF9A-4B26-8D2E-E7F44D769E94}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:v>RL Score</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataLabels>
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+          </cx:dataLabels>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling max="1"/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
   </cx:chart>
 </cx:chartSpace>
 </file>
@@ -1378,6 +1526,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="370">
   <cs:axisTitle>
@@ -3504,6 +3692,521 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
@@ -3789,6 +4492,89 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3B3ED83-7711-D981-C81F-796C9C605537}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5265420" y="369570"/>
+              <a:ext cx="22844760" cy="12485370"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4885,20 +5671,20 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
     </row>
     <row r="6" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
@@ -5140,12 +5926,12 @@
       </c>
     </row>
     <row r="25" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
@@ -5399,246 +6185,486 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{925387E9-A761-43C7-A3F6-A7F0D6717FC1}">
-  <dimension ref="B5:E26"/>
+  <dimension ref="A5:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="AS14" sqref="AS14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="16.21875" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="13.5546875" customWidth="1"/>
     <col min="4" max="4" width="14.88671875" customWidth="1"/>
     <col min="5" max="5" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B5" s="17" t="s">
+    <row r="5" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B5" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="16" t="s">
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
       <c r="B7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1">
+        <v>0.96</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E7" s="1">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1">
+        <v>0.94</v>
+      </c>
       <c r="D8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E8" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1">
+        <v>0.97</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E9" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
+      <c r="C11" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="1" t="s">
+      <c r="E11" s="1">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
+      <c r="C12" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="1" t="s">
+      <c r="E12" s="1">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1" t="s">
+      <c r="C13" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
+      <c r="E13" s="1">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1" t="s">
+      <c r="C14" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="1" t="s">
+      <c r="E14" s="1">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1" t="s">
+      <c r="C16" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="1" t="s">
+      <c r="E16" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1" t="s">
+      <c r="C17" s="1">
+        <v>0.9355</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="1" t="s">
+      <c r="E17" s="1">
+        <v>0.7097</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1" t="s">
+      <c r="C18" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" s="1" t="s">
+      <c r="E18" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1" t="s">
+      <c r="C19" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
+      <c r="E19" s="1">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1" t="s">
+      <c r="C21" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="1" t="s">
+      <c r="E21" s="1">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1" t="s">
+      <c r="C22" s="1">
+        <v>0.97219999999999995</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="1" t="s">
+      <c r="E22" s="1">
+        <v>0.86109999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1" t="s">
+      <c r="C23" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="1" t="s">
+      <c r="E23" s="1">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1" t="s">
+      <c r="C24" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E24" s="1">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.84</v>
+      </c>
       <c r="D25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="1"/>
+      <c r="C26" s="1">
+        <v>0.93</v>
+      </c>
       <c r="D26" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="1"/>
+      <c r="E26" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.96550000000000002</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.8276</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.76</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.57999999999999996</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update excel files for analysys
</commit_message>
<xml_diff>
--- a/Analysis/BGLStats.xlsx
+++ b/Analysis/BGLStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\MGL870-TP2-Remise\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D04511-2ABC-4B51-A298-CEED162758DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBE086B-DE14-45DD-8BB1-C308C68B82C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,19 +21,20 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Stats!$B$6:$B$46</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Stats!$C$6:$C$46</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'RF+RL Traning'!$E$6</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'RF+RL Traning'!$E$7:$E$36</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'RF+RL Traning'!$B$7:$B$36</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'RF+RL Traning'!$C$6</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'RF+RL Traning'!$C$7:$C$36</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'RF+RL Traning'!$E$6:$E$35</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'RF+RL Traning'!$C$5</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'RF+RL Traning'!$C$6:$C$35</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'RF+RL Traning'!$D$6:$D$35</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'RF+RL Traning'!$E$5</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'RF+RL Traning'!$E$6:$E$35</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Stats!$B$6:$B$46</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Stats!$C$6:$C$46</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">'Stats 2'!$B$6:$B$46</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">'Stats 2'!$D$6:$D$46</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'RF+RL Traning'!$B$7:$B$36</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'RF+RL Traning'!$C$6</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'RF+RL Traning'!$C$7:$C$36</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'RF+RL Traning'!$D$7:$D$36</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'RF+RL Traning'!$C$5</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'RF+RL Traning'!$C$6:$C$35</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'RF+RL Traning'!$D$6:$D$35</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'RF+RL Traning'!$E$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="69">
   <si>
     <t>APPALLOC</t>
   </si>
@@ -258,6 +259,12 @@
   <si>
     <t>1000 th 50</t>
   </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>RL</t>
+  </si>
 </sst>
 </file>
 
@@ -351,19 +358,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -421,9 +428,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -433,7 +437,13 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1253,18 +1263,18 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.12</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1290,7 +1300,7 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr/>
+              <a:defRPr sz="800"/>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
@@ -1322,31 +1332,66 @@
         <cx:series layoutId="boxWhisker" uniqueId="{081407F1-00F4-4940-A706-C1CA52CC8A8E}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.7</cx:f>
+              <cx:f>_xlchart.v1.11</cx:f>
               <cx:v>RF Score</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataLabels>
+            <cx:txPr>
+              <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" rtl="0">
+                  <a:defRPr sz="800" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US" sz="800"/>
+              </a:p>
+            </cx:txPr>
             <cx:visibility seriesName="0" categoryName="0" value="1"/>
           </cx:dataLabels>
           <cx:dataId val="0"/>
           <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
         <cx:series layoutId="boxWhisker" uniqueId="{00000001-DF9A-4B26-8D2E-E7F44D769E94}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:f>_xlchart.v1.14</cx:f>
               <cx:v>RL Score</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataLabels>
+            <cx:txPr>
+              <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" rtl="0">
+                  <a:defRPr sz="800" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US" sz="800"/>
+              </a:p>
+            </cx:txPr>
             <cx:visibility seriesName="0" categoryName="0" value="1"/>
           </cx:dataLabels>
           <cx:dataId val="1"/>
           <cx:layoutPr>
+            <cx:visibility meanLine="1"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
@@ -1354,14 +1399,66 @@
       <cx:axis id="0">
         <cx:catScaling gapWidth="1"/>
         <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1800" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1800"/>
+          </a:p>
+        </cx:txPr>
       </cx:axis>
       <cx:axis id="1">
         <cx:valScaling max="1"/>
         <cx:majorGridlines/>
         <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1800" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1800"/>
+          </a:p>
+        </cx:txPr>
       </cx:axis>
     </cx:plotArea>
-    <cx:legend pos="t" align="ctr" overlay="0"/>
+    <cx:legend pos="t" align="ctr" overlay="0">
+      <cx:txPr>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1800" b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="595959"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1800"/>
+        </a:p>
+      </cx:txPr>
+    </cx:legend>
   </cx:chart>
 </cx:chartSpace>
 </file>
@@ -4504,7 +4601,7 @@
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -4542,7 +4639,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="5265420" y="369570"/>
-              <a:ext cx="22844760" cy="12485370"/>
+              <a:ext cx="22844760" cy="12302490"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -5671,20 +5768,20 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
     </row>
     <row r="6" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
@@ -5926,12 +6023,12 @@
       </c>
     </row>
     <row r="25" spans="2:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
@@ -6185,10 +6282,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{925387E9-A761-43C7-A3F6-A7F0D6717FC1}">
-  <dimension ref="A5:E36"/>
+  <dimension ref="A4:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="AS14" sqref="AS14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6200,469 +6297,502 @@
     <col min="5" max="5" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B5" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
+    <row r="4" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B4" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>58</v>
+      <c r="A6" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.96</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.64</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>62</v>
-      </c>
+      <c r="A7" s="17"/>
       <c r="B7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
+      <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="1">
+        <v>-0.79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="17"/>
+      <c r="B10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="1">
-        <v>0.96</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="C11" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="1">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
+      <c r="E11" s="1">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C12" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="17"/>
+      <c r="B14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="1">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="17"/>
+      <c r="B15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.9355</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.7097</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="17"/>
+      <c r="B17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
+      <c r="B18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="17"/>
+      <c r="B19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="1">
+        <v>-0.33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="17"/>
+      <c r="B20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.97219999999999995</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.86109999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="17"/>
+      <c r="B22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="17"/>
+      <c r="B23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="1">
         <v>0.94</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="17"/>
+      <c r="B24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="17"/>
+      <c r="B25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.96550000000000002</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.8276</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="17"/>
+      <c r="B27" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
+      <c r="C27" s="1">
+        <v>0.89</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="17"/>
+      <c r="B28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="1">
-        <v>0.97</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C28" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="1">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
+      <c r="E28" s="1">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="17"/>
+      <c r="B29" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="C29" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="1">
-        <v>0.79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="1" t="s">
+      <c r="E29" s="1">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="17"/>
+      <c r="B30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="1">
-        <v>0.97</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="C30" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="1">
-        <v>0.67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="1" t="s">
+      <c r="E30" s="1">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="1">
-        <v>0.92</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="C31" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E31" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="17"/>
+      <c r="B32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="1">
         <v>0.76</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="1">
-        <v>0.78</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B14" s="1" t="s">
+      <c r="E32" s="1">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="17"/>
+      <c r="B33" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="1">
-        <v>0.89</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="C33" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="1">
-        <v>0.67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="1" t="s">
+      <c r="E33" s="1">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="17"/>
+      <c r="B34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="1">
-        <v>0.65</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="C34" s="1">
+        <v>0.26</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="1">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="1" t="s">
+      <c r="E34" s="1">
+        <v>-0.84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="17"/>
+      <c r="B35" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="1">
-        <v>0.88</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="C35" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0.9355</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0.7097</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0.79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B20" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="1">
-        <v>0.95</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0.97219999999999995</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0.86109999999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0.88</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="1">
-        <v>0.94</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="1">
-        <v>0.69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="1">
-        <v>0.84</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E25" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="1">
-        <v>0.93</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E26" s="1">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="1">
-        <v>0.96550000000000002</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="1">
-        <v>0.8276</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B28" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="1">
-        <v>0.89</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E28" s="1">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B29" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="1">
-        <v>0.94</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" s="1">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B30" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="1">
-        <v>0.84</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" s="1">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B31" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C31" s="1">
-        <v>0.94</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E31" s="1">
-        <v>0.62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="1">
-        <v>0.84</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E32" s="1">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B33" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="1">
-        <v>0.76</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E33" s="1">
-        <v>0.41</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B34" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="1">
-        <v>0.88</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E34" s="1">
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B35" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" s="1">
-        <v>0.26</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="E35" s="1">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C36" s="1">
-        <v>0.87</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E36" s="1">
         <v>0.57999999999999996</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B5:E5"/>
+  <mergeCells count="8">
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A21:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Add script to process bgl data
</commit_message>
<xml_diff>
--- a/Analysis/BGLStats.xlsx
+++ b/Analysis/BGLStats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\MGL870-TP2-Remise\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C95FA47-9276-4B0F-9BAE-E8786C58140C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CFD6A48-A52E-42EA-B5BA-926DB735CF9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,8 @@
     <sheet name="AUC" sheetId="3" r:id="rId3"/>
     <sheet name="RF+RL Traning" sheetId="4" r:id="rId4"/>
     <sheet name="Interpretation RF" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
+    <sheet name="RF+RL Traning Aggregation" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Stats!$B$6:$B$46</definedName>
@@ -27,13 +28,15 @@
     <definedName name="_xlchart.v1.11" hidden="1">'Interpretation RF'!$D$10:$E$27</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">'Interpretation RF'!$F$10:$F$27</definedName>
     <definedName name="_xlchart.v1.13" hidden="1">'Interpretation RF'!$F$9</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$D$9:$E$26</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$F$8</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$F$9:$F$26</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$D$9:$E$26</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$F$8</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$F$9:$F$26</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'RF+RL Traning Aggregation'!$C$5</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'RF+RL Traning Aggregation'!$C$6:$C$35</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'RF+RL Traning Aggregation'!$D$6:$D$35</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'RF+RL Traning Aggregation'!$E$5</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'RF+RL Traning Aggregation'!$E$6:$E$35</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$D$9:$E$26</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Stats!$B$6:$B$46</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$F$8</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$F$9:$F$26</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Stats!$C$6:$C$46</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">'Stats 2'!$B$6:$B$46</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">'Stats 2'!$D$6:$D$46</definedName>
@@ -63,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="101">
   <si>
     <t>APPALLOC</t>
   </si>
@@ -348,6 +351,24 @@
   </si>
   <si>
     <t>BGL - RL 5M - KERNDTLB</t>
+  </si>
+  <si>
+    <t>5min</t>
+  </si>
+  <si>
+    <t>10 min</t>
+  </si>
+  <si>
+    <t>20 min</t>
+  </si>
+  <si>
+    <t>30 min</t>
+  </si>
+  <si>
+    <t>45 min</t>
+  </si>
+  <si>
+    <t>60 min</t>
   </si>
 </sst>
 </file>
@@ -1178,10 +1199,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1260,10 +1281,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1654,10 +1675,203 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.17</cx:f>
+        <cx:f>_xlchart.v1.16</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
+        <cx:f>_xlchart.v1.15</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.16</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.18</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Performances de RF et RL - BGL 5M - 80%-20% - Aggrégations</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{081407F1-00F4-4940-A706-C1CA52CC8A8E}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:v>RF Score</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataLabels>
+            <cx:txPr>
+              <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" rtl="0">
+                  <a:defRPr sz="800" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US" sz="800"/>
+              </a:p>
+            </cx:txPr>
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000001-DF9A-4B26-8D2E-E7F44D769E94}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.17</cx:f>
+              <cx:v>RL Score</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataLabels>
+            <cx:txPr>
+              <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" rtl="0">
+                  <a:defRPr sz="800" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US" sz="800"/>
+              </a:p>
+            </cx:txPr>
+            <cx:visibility seriesName="0" categoryName="0" value="1"/>
+          </cx:dataLabels>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1800" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1800"/>
+          </a:p>
+        </cx:txPr>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling max="1"/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+        <cx:txPr>
+          <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr sz="1800" b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US" sz="1800"/>
+          </a:p>
+        </cx:txPr>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0">
+      <cx:txPr>
+        <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1800" b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="595959"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1800"/>
+        </a:p>
+      </cx:txPr>
+    </cx:legend>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx7.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
         <cx:f>_xlchart.v1.19</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.21</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1668,7 +1882,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{7BA02CB4-84B4-4E92-A9C7-63ABE1B94395}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.18</cx:f>
+              <cx:f>_xlchart.v1.20</cx:f>
               <cx:v>Importance [0-1]</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1976,6 +2190,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="370">
   <cs:axisTitle>
@@ -5138,6 +5392,521 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6102,16 +6871,99 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>72390</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDCB5CD9-3512-4CE7-A703-13FE928FE1FB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5265420" y="369570"/>
+              <a:ext cx="22844760" cy="12302490"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -6147,7 +6999,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8793480" y="1718310"/>
+              <a:off x="7459980" y="1024890"/>
               <a:ext cx="8854440" cy="5817870"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -8590,11 +9442,530 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{596A295A-EAE6-4AB9-9E85-00E8D71D4D76}">
+  <dimension ref="A4:E35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AR40" sqref="AR40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.21875" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B4" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.77849999999999997</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.80279999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="18"/>
+      <c r="B7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.79</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="18"/>
+      <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="18"/>
+      <c r="B9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="18"/>
+      <c r="B10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.79600000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="18"/>
+      <c r="B12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="18"/>
+      <c r="B13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="18"/>
+      <c r="B14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="18"/>
+      <c r="B15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.70699999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="18"/>
+      <c r="B17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="18"/>
+      <c r="B18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.81</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="18"/>
+      <c r="B19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="1">
+        <v>-0.18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="18"/>
+      <c r="B20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.83160000000000001</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.70409999999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="18"/>
+      <c r="B22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="18"/>
+      <c r="B23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="18"/>
+      <c r="B24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.31</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="1">
+        <v>-0.21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="18"/>
+      <c r="B25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.73599999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="18"/>
+      <c r="B27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="18"/>
+      <c r="B28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.81</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="18"/>
+      <c r="B29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.21</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="1">
+        <v>-0.09</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="18"/>
+      <c r="B30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.82740000000000002</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.70830000000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="18"/>
+      <c r="B32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="18"/>
+      <c r="B33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="18"/>
+      <c r="B34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" s="1">
+        <v>-0.22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="18"/>
+      <c r="B35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0.68</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A21:A25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B098052-7642-45FE-9F68-764DCB8FC916}">
   <dimension ref="C7:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>